<commit_message>
update the team member report
</commit_message>
<xml_diff>
--- a/documents/Deliverable_4/FlyingMongeese_Deliverable_4_Team_Member_Report.xlsx
+++ b/documents/Deliverable_4/FlyingMongeese_Deliverable_4_Team_Member_Report.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aaron/Documents/GitHub/Software2project/documents/Deliverable_3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carolyn\Documents\GitHub\Software2project\documents\Deliverable_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEECF362-63B9-4813-9052-95BC98543621}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="440" windowWidth="21600" windowHeight="15100" activeTab="3"/>
+    <workbookView xWindow="936" yWindow="444" windowWidth="21600" windowHeight="15096" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mayur" sheetId="1" r:id="rId1"/>
@@ -24,18 +25,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="188">
   <si>
     <t>Week of</t>
   </si>
@@ -602,11 +603,35 @@
   <si>
     <t>Week of 4/9/2018</t>
   </si>
+  <si>
+    <t xml:space="preserve">make all the documents formalized </t>
+  </si>
+  <si>
+    <t>make all the documents formalized</t>
+  </si>
+  <si>
+    <t>Week of 4/16/2018</t>
+  </si>
+  <si>
+    <t>Week of 4/23/2018</t>
+  </si>
+  <si>
+    <t>finalize all the documents</t>
+  </si>
+  <si>
+    <t>finish personal team report and kanban board</t>
+  </si>
+  <si>
+    <t>finish personal team report and kanban Board</t>
+  </si>
+  <si>
+    <t>finish team report and kanban board</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -789,16 +814,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1124,40 +1149,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="C38" sqref="C38:D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5" customWidth="1"/>
-    <col min="2" max="2" width="34.5" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" customWidth="1"/>
-    <col min="4" max="4" width="33.5" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" customWidth="1"/>
+    <col min="3" max="3" width="27.77734375" customWidth="1"/>
+    <col min="4" max="4" width="33.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1171,7 +1196,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1185,7 +1210,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1199,7 +1224,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="45.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1213,7 +1238,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -1227,7 +1252,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -1241,31 +1266,31 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-    </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="20"/>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -1279,7 +1304,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
@@ -1293,7 +1318,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -1307,7 +1332,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -1321,7 +1346,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
@@ -1335,7 +1360,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
@@ -1349,31 +1374,31 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="21" t="s">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-    </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="20"/>
-    </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>1</v>
       </c>
@@ -1387,7 +1412,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -1401,7 +1426,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -1415,7 +1440,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -1429,7 +1454,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
@@ -1443,7 +1468,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
@@ -1457,31 +1482,31 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
     </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="19" t="s">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-    </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="20" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20" t="s">
+      <c r="B29" s="21"/>
+      <c r="C29" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="20"/>
-    </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
@@ -1495,7 +1520,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>2</v>
       </c>
@@ -1509,7 +1534,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -1523,7 +1548,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -1537,7 +1562,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -1551,7 +1576,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -1565,31 +1590,31 @@
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="s">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-    </row>
-    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="20" t="s">
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20" t="s">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="D38" s="20"/>
-    </row>
-    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>1</v>
       </c>
@@ -1603,7 +1628,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>2</v>
       </c>
@@ -1617,7 +1642,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -1631,7 +1656,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -1645,7 +1670,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>5</v>
       </c>
@@ -1659,7 +1684,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>6</v>
       </c>
@@ -1673,31 +1698,31 @@
         <v>172</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
     </row>
-    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="21" t="s">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-    </row>
-    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="22" t="s">
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="20" t="s">
+      <c r="B47" s="20"/>
+      <c r="C47" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D47" s="20"/>
-    </row>
-    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>1</v>
       </c>
@@ -1711,7 +1736,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>2</v>
       </c>
@@ -1721,7 +1746,7 @@
       </c>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -1731,7 +1756,7 @@
       </c>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -1741,7 +1766,7 @@
       </c>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>5</v>
       </c>
@@ -1751,7 +1776,7 @@
       </c>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>6</v>
       </c>
@@ -1763,662 +1788,9 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:D29"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D53"/>
-  <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38:D38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="25.5" customWidth="1"/>
-    <col min="2" max="2" width="29.5" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="27.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-    </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="20"/>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-    </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-    </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="20"/>
-    </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-    </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-    </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="D29" s="20"/>
-    </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-    </row>
-    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-    </row>
-    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="D38" s="20"/>
-    </row>
-    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-    </row>
-    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-    </row>
-    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="20"/>
-    </row>
-    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D49" s="11"/>
-    </row>
-    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D50" s="11"/>
-    </row>
-    <row r="51" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="11"/>
-    </row>
-    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="11"/>
-    </row>
-    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="18">
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -2431,52 +1803,705 @@
     <mergeCell ref="A46:D46"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D53"/>
+  <sheetViews>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38:D38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+    </row>
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="20"/>
+      <c r="C47" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="11"/>
+      <c r="C49" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="11"/>
+    </row>
+    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="11"/>
+      <c r="C50" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="11"/>
+    </row>
+    <row r="51" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="11"/>
+      <c r="C51" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="11"/>
+    </row>
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="11"/>
+      <c r="C52" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="11"/>
+    </row>
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" s="11"/>
+      <c r="C53" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C38" sqref="C38:D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="29.5" customWidth="1"/>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="34.5" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="34.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-    </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -2490,7 +2515,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -2504,7 +2529,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -2520,7 +2545,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -2536,7 +2561,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -2552,7 +2577,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -2566,31 +2591,31 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
     </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-    </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="20"/>
-    </row>
-    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -2604,7 +2629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
@@ -2618,7 +2643,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -2634,7 +2659,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -2650,7 +2675,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
@@ -2666,7 +2691,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
@@ -2682,31 +2707,31 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
     </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="21" t="s">
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-    </row>
-    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="20"/>
-    </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>1</v>
       </c>
@@ -2720,7 +2745,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -2734,7 +2759,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -2748,7 +2773,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -2762,7 +2787,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
@@ -2776,7 +2801,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
@@ -2790,31 +2815,31 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
     </row>
-    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="21" t="s">
+    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-    </row>
-    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="20" t="s">
+      <c r="B29" s="20"/>
+      <c r="C29" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="20"/>
-    </row>
-    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>1</v>
       </c>
@@ -2828,7 +2853,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>2</v>
       </c>
@@ -2842,7 +2867,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -2856,7 +2881,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -2870,7 +2895,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>5</v>
       </c>
@@ -2884,7 +2909,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>6</v>
       </c>
@@ -2898,31 +2923,31 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="14"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
     </row>
-    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="21" t="s">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-    </row>
-    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="20" t="s">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20" t="s">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="D38" s="20"/>
-    </row>
-    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>1</v>
       </c>
@@ -2936,7 +2961,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>2</v>
       </c>
@@ -2950,7 +2975,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -2964,7 +2989,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -2978,7 +3003,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>5</v>
       </c>
@@ -2992,7 +3017,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>6</v>
       </c>
@@ -3006,31 +3031,31 @@
         <v>154</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
     </row>
-    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="21" t="s">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-    </row>
-    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="22" t="s">
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="20" t="s">
+      <c r="B47" s="20"/>
+      <c r="C47" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D47" s="20"/>
-    </row>
-    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>1</v>
       </c>
@@ -3044,7 +3069,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>2</v>
       </c>
@@ -3054,7 +3079,7 @@
       </c>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -3064,7 +3089,7 @@
       </c>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -3074,7 +3099,7 @@
       </c>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>5</v>
       </c>
@@ -3084,7 +3109,7 @@
       </c>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>6</v>
       </c>
@@ -3096,12 +3121,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -3114,47 +3133,53 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="C38" sqref="C38:D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.5" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="29.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -3168,7 +3193,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -3182,7 +3207,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -3196,7 +3221,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -3210,7 +3235,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -3224,7 +3249,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -3238,31 +3263,31 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-    </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="20"/>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
@@ -3276,7 +3301,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
@@ -3290,7 +3315,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -3304,7 +3329,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -3318,7 +3343,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -3332,7 +3357,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>6</v>
       </c>
@@ -3346,31 +3371,31 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-    </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="20"/>
-    </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>1</v>
       </c>
@@ -3384,7 +3409,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -3398,7 +3423,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -3412,7 +3437,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -3426,7 +3451,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -3440,7 +3465,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -3454,31 +3479,31 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="19" t="s">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-    </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="20" t="s">
+      <c r="B29" s="20"/>
+      <c r="C29" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="20"/>
-    </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
@@ -3492,7 +3517,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>2</v>
       </c>
@@ -3506,7 +3531,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -3520,7 +3545,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -3534,7 +3559,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -3548,7 +3573,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -3562,31 +3587,31 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="s">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-    </row>
-    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="20" t="s">
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20" t="s">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="D38" s="20"/>
-    </row>
-    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>1</v>
       </c>
@@ -3600,7 +3625,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>2</v>
       </c>
@@ -3614,7 +3639,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -3628,7 +3653,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -3642,7 +3667,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>5</v>
       </c>
@@ -3656,7 +3681,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>6</v>
       </c>
@@ -3670,31 +3695,31 @@
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="19" t="s">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-    </row>
-    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="20" t="s">
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20" t="s">
+      <c r="B47" s="21"/>
+      <c r="C47" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D47" s="20"/>
-    </row>
-    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>1</v>
       </c>
@@ -3708,7 +3733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>2</v>
       </c>
@@ -3722,7 +3747,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -3732,7 +3757,7 @@
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -3742,7 +3767,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>5</v>
       </c>
@@ -3752,7 +3777,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>6</v>
       </c>
@@ -3764,12 +3789,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -3782,6 +3801,12 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3789,40 +3814,40 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C38" sqref="C38:D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="40.83203125" customWidth="1"/>
-    <col min="3" max="3" width="22.5" customWidth="1"/>
-    <col min="4" max="4" width="40.5" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="40.77734375" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="40.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -3836,7 +3861,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -3850,7 +3875,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -3864,7 +3889,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -3878,7 +3903,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -3892,7 +3917,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -3906,31 +3931,31 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-    </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="20"/>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
@@ -3944,7 +3969,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
@@ -3958,7 +3983,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="78" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -3972,7 +3997,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -3986,7 +4011,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -4000,7 +4025,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>6</v>
       </c>
@@ -4014,31 +4039,31 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-    </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="20"/>
-    </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>1</v>
       </c>
@@ -4052,7 +4077,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -4066,7 +4091,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -4080,7 +4105,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -4094,7 +4119,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -4108,7 +4133,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -4122,31 +4147,31 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="19" t="s">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-    </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="20" t="s">
+      <c r="B29" s="20"/>
+      <c r="C29" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="20"/>
-    </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
@@ -4160,7 +4185,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>2</v>
       </c>
@@ -4174,7 +4199,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -4188,7 +4213,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -4202,7 +4227,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="78" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -4216,7 +4241,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -4230,31 +4255,31 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="s">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-    </row>
-    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="20" t="s">
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20" t="s">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="D38" s="20"/>
-    </row>
-    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>1</v>
       </c>
@@ -4268,7 +4293,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>2</v>
       </c>
@@ -4282,7 +4307,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -4296,7 +4321,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="78" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -4310,7 +4335,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>5</v>
       </c>
@@ -4324,7 +4349,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>6</v>
       </c>
@@ -4334,31 +4359,31 @@
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="19" t="s">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-    </row>
-    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="20" t="s">
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20" t="s">
+      <c r="B47" s="21"/>
+      <c r="C47" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D47" s="20"/>
-    </row>
-    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>1</v>
       </c>
@@ -4372,7 +4397,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>2</v>
       </c>
@@ -4382,7 +4407,7 @@
       </c>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -4392,7 +4417,7 @@
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -4402,7 +4427,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>5</v>
       </c>
@@ -4412,7 +4437,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>6</v>
       </c>
@@ -4424,12 +4449,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -4442,6 +4461,12 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4449,40 +4474,40 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38:D38"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
     <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
-    <col min="4" max="4" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" customWidth="1"/>
+    <col min="4" max="4" width="40.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -4496,7 +4521,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -4510,7 +4535,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -4524,7 +4549,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -4538,7 +4563,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -4552,7 +4577,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -4566,13 +4591,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>8</v>
       </c>
@@ -4580,17 +4605,17 @@
       <c r="C10" s="24"/>
       <c r="D10" s="25"/>
     </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="20"/>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -4604,7 +4629,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
@@ -4618,7 +4643,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -4632,7 +4657,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -4646,7 +4671,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
@@ -4660,7 +4685,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
@@ -4674,31 +4699,31 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="21" t="s">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-    </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="20"/>
-    </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>1</v>
       </c>
@@ -4712,7 +4737,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -4726,7 +4751,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -4740,7 +4765,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -4754,7 +4779,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
@@ -4768,7 +4793,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
@@ -4782,31 +4807,31 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
     </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="19" t="s">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-    </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="20" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20" t="s">
+      <c r="B29" s="21"/>
+      <c r="C29" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="20"/>
-    </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
@@ -4820,7 +4845,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>2</v>
       </c>
@@ -4834,7 +4859,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -4848,7 +4873,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -4862,7 +4887,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -4876,7 +4901,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -4890,31 +4915,31 @@
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="21" t="s">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-    </row>
-    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="20" t="s">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20" t="s">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="D38" s="20"/>
-    </row>
-    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>1</v>
       </c>
@@ -4928,7 +4953,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>2</v>
       </c>
@@ -4942,7 +4967,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -4956,7 +4981,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -4970,7 +4995,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>5</v>
       </c>
@@ -4984,7 +5009,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>6</v>
       </c>
@@ -4998,31 +5023,31 @@
         <v>178</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
     </row>
-    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="21" t="s">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-    </row>
-    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="20"/>
-    </row>
-    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="B47" s="20"/>
+      <c r="C47" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>1</v>
       </c>
@@ -5036,64 +5061,78 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B49" s="8"/>
+      <c r="B49" s="8" t="s">
+        <v>123</v>
+      </c>
       <c r="C49" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D49" s="8"/>
-    </row>
-    <row r="50" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D49" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B50" s="8"/>
+      <c r="B50" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="C50" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D50" s="8"/>
-    </row>
-    <row r="51" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D50" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B51" s="8"/>
+      <c r="B51" s="8" t="s">
+        <v>185</v>
+      </c>
       <c r="C51" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="8"/>
-    </row>
-    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D51" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="8"/>
+      <c r="B52" s="8" t="s">
+        <v>187</v>
+      </c>
       <c r="C52" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="8"/>
-    </row>
-    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D52" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B53" s="8"/>
+      <c r="B53" s="8" t="s">
+        <v>184</v>
+      </c>
       <c r="C53" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="8"/>
+      <c r="D53" s="8" t="s">
+        <v>184</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -5106,6 +5145,12 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished Team member report
</commit_message>
<xml_diff>
--- a/documents/Deliverable_4/FlyingMongeese_Deliverable_4_Team_Member_Report.xlsx
+++ b/documents/Deliverable_4/FlyingMongeese_Deliverable_4_Team_Member_Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arsga\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayur Bhakta\Documents\GitHub\Software2project\documents\Deliverable_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38B0EC8-699E-4F2C-9625-A25097F714BD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5305518-D892-4141-8098-2715059D7FA8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12180" windowHeight="6280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12180" windowHeight="6276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mayur" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="196">
   <si>
     <t>Week of</t>
   </si>
@@ -632,6 +632,27 @@
   </si>
   <si>
     <t>Documentation Final updates</t>
+  </si>
+  <si>
+    <t>Minor fixes on the application.
+Fix Domain-design document.</t>
+  </si>
+  <si>
+    <t>Understanding the behavior of UML arrows.</t>
+  </si>
+  <si>
+    <t>Finish all remaining documents before deliverable 4 due date.</t>
+  </si>
+  <si>
+    <t>None.</t>
+  </si>
+  <si>
+    <t>Finished up domain-design document.
+Created misuse cases and description for them.
+Finalize updating remaining documents.</t>
+  </si>
+  <si>
+    <t>Week of 4/30/2018</t>
   </si>
 </sst>
 </file>
@@ -820,16 +841,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1158,37 +1179,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38:D38"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.453125" customWidth="1"/>
-    <col min="2" max="2" width="34.453125" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" customWidth="1"/>
-    <col min="4" max="4" width="33.453125" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" customWidth="1"/>
+    <col min="3" max="3" width="27.77734375" customWidth="1"/>
+    <col min="4" max="4" width="36.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="22" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1202,7 +1223,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1216,7 +1237,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1230,7 +1251,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="45.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1244,7 +1265,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -1258,7 +1279,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -1272,31 +1293,31 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="20"/>
-    </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -1310,7 +1331,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
@@ -1324,7 +1345,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -1338,7 +1359,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -1352,7 +1373,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
@@ -1366,7 +1387,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
@@ -1380,31 +1401,31 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="20" t="s">
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="20"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>1</v>
       </c>
@@ -1418,7 +1439,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -1432,7 +1453,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -1446,7 +1467,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -1460,7 +1481,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
@@ -1474,7 +1495,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
@@ -1488,31 +1509,31 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A28" s="19" t="s">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="20" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20" t="s">
+      <c r="B29" s="21"/>
+      <c r="C29" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="20"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
@@ -1526,7 +1547,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>2</v>
       </c>
@@ -1540,7 +1561,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -1554,7 +1575,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -1568,7 +1589,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -1582,7 +1603,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -1596,31 +1617,31 @@
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A37" s="19" t="s">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-    </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="20" t="s">
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20" t="s">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="D38" s="20"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>1</v>
       </c>
@@ -1634,7 +1655,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>2</v>
       </c>
@@ -1648,7 +1669,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -1662,7 +1683,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -1676,7 +1697,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>5</v>
       </c>
@@ -1690,7 +1711,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>6</v>
       </c>
@@ -1704,31 +1725,31 @@
         <v>172</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
     </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A46" s="21" t="s">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-    </row>
-    <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="20"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="B47" s="20"/>
+      <c r="C47" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>1</v>
       </c>
@@ -1742,714 +1763,81 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B49" s="8"/>
+      <c r="B49" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="C49" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D49" s="8"/>
-    </row>
-    <row r="50" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D49" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B50" s="8"/>
+      <c r="B50" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="C50" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D50" s="8"/>
-    </row>
-    <row r="51" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="D50" s="17" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B51" s="8"/>
+      <c r="B51" s="17" t="s">
+        <v>192</v>
+      </c>
       <c r="C51" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="8"/>
-    </row>
-    <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D51" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="8"/>
+      <c r="B52" s="17" t="s">
+        <v>191</v>
+      </c>
       <c r="C52" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="8"/>
-    </row>
-    <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D52" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B53" s="8"/>
+      <c r="B53" s="17" t="s">
+        <v>191</v>
+      </c>
       <c r="C53" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="8"/>
+      <c r="D53" s="8" t="s">
+        <v>193</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:D29"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D53"/>
-  <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38:D38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="25.453125" customWidth="1"/>
-    <col min="2" max="2" width="29.453125" customWidth="1"/>
-    <col min="3" max="3" width="26.453125" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="20"/>
-    </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="20"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="62" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A25" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-    </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A28" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="D29" s="20"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-    </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A37" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-    </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="D38" s="20"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-    </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A46" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-    </row>
-    <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="20"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D49" s="11"/>
-    </row>
-    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D50" s="11"/>
-    </row>
-    <row r="51" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="11"/>
-    </row>
-    <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="11"/>
-    </row>
-    <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="18">
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -2462,12 +1850,665 @@
     <mergeCell ref="A46:D46"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D53"/>
+  <sheetViews>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38:D38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+    </row>
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="20"/>
+      <c r="C47" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="11"/>
+      <c r="C49" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="11"/>
+    </row>
+    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="11"/>
+      <c r="C50" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="11"/>
+    </row>
+    <row r="51" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="11"/>
+      <c r="C51" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="11"/>
+    </row>
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="11"/>
+      <c r="C52" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="11"/>
+    </row>
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" s="11"/>
+      <c r="C53" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2477,37 +2518,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="29.453125" customWidth="1"/>
-    <col min="3" max="3" width="20.453125" customWidth="1"/>
-    <col min="4" max="4" width="34.453125" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="34.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="22" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -2521,7 +2562,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -2535,7 +2576,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -2551,7 +2592,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -2567,7 +2608,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -2583,7 +2624,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -2597,31 +2638,31 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="20"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -2635,7 +2676,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
@@ -2649,7 +2690,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -2665,7 +2706,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -2681,7 +2722,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
@@ -2697,7 +2738,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
@@ -2713,31 +2754,31 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
     </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="20" t="s">
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="20"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>1</v>
       </c>
@@ -2751,7 +2792,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -2765,7 +2806,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -2779,7 +2820,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -2793,7 +2834,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
@@ -2807,7 +2848,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
@@ -2821,31 +2862,31 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
     </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="A28" s="21" t="s">
+    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="22" t="s">
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="20" t="s">
+      <c r="B29" s="20"/>
+      <c r="C29" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="20"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>1</v>
       </c>
@@ -2859,7 +2900,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>2</v>
       </c>
@@ -2873,7 +2914,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -2887,7 +2928,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -2901,7 +2942,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>5</v>
       </c>
@@ -2915,7 +2956,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>6</v>
       </c>
@@ -2929,31 +2970,31 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="14"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A37" s="21" t="s">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-    </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="20" t="s">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20" t="s">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="D38" s="20"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>1</v>
       </c>
@@ -2967,7 +3008,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>2</v>
       </c>
@@ -2981,7 +3022,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -2995,7 +3036,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -3009,7 +3050,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>5</v>
       </c>
@@ -3023,7 +3064,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>6</v>
       </c>
@@ -3037,31 +3078,31 @@
         <v>154</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
     </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A46" s="21" t="s">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-    </row>
-    <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="22" t="s">
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="20" t="s">
+      <c r="B47" s="20"/>
+      <c r="C47" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="D47" s="20"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>1</v>
       </c>
@@ -3075,7 +3116,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>2</v>
       </c>
@@ -3089,7 +3130,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -3103,7 +3144,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -3117,7 +3158,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>5</v>
       </c>
@@ -3131,7 +3172,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>6</v>
       </c>
@@ -3147,12 +3188,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -3165,6 +3200,12 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3178,34 +3219,34 @@
       <selection activeCell="C38" sqref="C38:D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.08984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.453125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.08984375" style="1"/>
+    <col min="1" max="1" width="29.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -3219,7 +3260,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -3233,7 +3274,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -3247,7 +3288,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -3261,7 +3302,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -3275,7 +3316,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -3289,31 +3330,31 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="20"/>
-    </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
@@ -3327,7 +3368,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
@@ -3341,7 +3382,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -3355,7 +3396,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -3369,7 +3410,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -3383,7 +3424,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>6</v>
       </c>
@@ -3397,31 +3438,31 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A19" s="19" t="s">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="20" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="20"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>1</v>
       </c>
@@ -3435,7 +3476,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -3449,7 +3490,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -3463,7 +3504,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -3477,7 +3518,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -3491,7 +3532,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -3505,31 +3546,31 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A28" s="19" t="s">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="22" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="20" t="s">
+      <c r="B29" s="20"/>
+      <c r="C29" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="20"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
@@ -3543,7 +3584,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>2</v>
       </c>
@@ -3557,7 +3598,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -3571,7 +3612,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -3585,7 +3626,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -3599,7 +3640,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -3613,31 +3654,31 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A37" s="19" t="s">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-    </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="20" t="s">
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20" t="s">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="D38" s="20"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>1</v>
       </c>
@@ -3651,7 +3692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>2</v>
       </c>
@@ -3665,7 +3706,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -3679,7 +3720,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -3693,7 +3734,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>5</v>
       </c>
@@ -3707,7 +3748,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>6</v>
       </c>
@@ -3721,31 +3762,31 @@
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A46" s="19" t="s">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-    </row>
-    <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="20" t="s">
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20" t="s">
+      <c r="B47" s="21"/>
+      <c r="C47" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D47" s="20"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>1</v>
       </c>
@@ -3759,7 +3800,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>2</v>
       </c>
@@ -3773,7 +3814,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -3783,7 +3824,7 @@
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -3793,7 +3834,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>5</v>
       </c>
@@ -3803,7 +3844,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>6</v>
       </c>
@@ -3815,12 +3856,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -3833,6 +3868,12 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3847,33 +3888,33 @@
       <selection activeCell="C38" sqref="C38:D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="2" max="2" width="40.81640625" customWidth="1"/>
-    <col min="3" max="3" width="22.453125" customWidth="1"/>
-    <col min="4" max="4" width="40.453125" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="40.77734375" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="40.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -3887,7 +3928,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -3901,7 +3942,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -3915,7 +3956,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -3929,7 +3970,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -3943,7 +3984,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -3957,31 +3998,31 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="20"/>
-    </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
@@ -3995,7 +4036,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
@@ -4009,7 +4050,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="78" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -4023,7 +4064,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="93" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -4037,7 +4078,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -4051,7 +4092,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>6</v>
       </c>
@@ -4065,31 +4106,31 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A19" s="19" t="s">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="20" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="20"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>1</v>
       </c>
@@ -4103,7 +4144,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -4117,7 +4158,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -4131,7 +4172,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -4145,7 +4186,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -4159,7 +4200,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -4173,31 +4214,31 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A28" s="19" t="s">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="22" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="20" t="s">
+      <c r="B29" s="20"/>
+      <c r="C29" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="20"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
@@ -4211,7 +4252,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>2</v>
       </c>
@@ -4225,7 +4266,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -4239,7 +4280,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -4253,7 +4294,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="78" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -4267,7 +4308,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -4281,31 +4322,31 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A37" s="19" t="s">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-    </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="20" t="s">
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20" t="s">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="D38" s="20"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>1</v>
       </c>
@@ -4319,7 +4360,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>2</v>
       </c>
@@ -4333,7 +4374,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -4347,7 +4388,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="78" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -4361,7 +4402,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>5</v>
       </c>
@@ -4375,7 +4416,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>6</v>
       </c>
@@ -4385,31 +4426,31 @@
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A46" s="19" t="s">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-    </row>
-    <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="20" t="s">
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20" t="s">
+      <c r="B47" s="21"/>
+      <c r="C47" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D47" s="20"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>1</v>
       </c>
@@ -4423,7 +4464,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>2</v>
       </c>
@@ -4433,7 +4474,7 @@
       </c>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -4443,7 +4484,7 @@
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -4453,7 +4494,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>5</v>
       </c>
@@ -4463,7 +4504,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>6</v>
       </c>
@@ -4475,12 +4516,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -4493,6 +4528,12 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4507,33 +4548,33 @@
       <selection activeCell="A47" sqref="A47:B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.453125" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
     <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" customWidth="1"/>
-    <col min="4" max="4" width="40.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" customWidth="1"/>
+    <col min="4" max="4" width="40.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -4547,7 +4588,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -4561,7 +4602,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -4575,7 +4616,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -4589,7 +4630,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -4603,7 +4644,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -4617,13 +4658,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>8</v>
       </c>
@@ -4631,17 +4672,17 @@
       <c r="C10" s="24"/>
       <c r="D10" s="25"/>
     </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="20"/>
-    </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -4655,7 +4696,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
@@ -4669,7 +4710,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -4683,7 +4724,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -4697,7 +4738,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
@@ -4711,7 +4752,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
@@ -4725,31 +4766,31 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="20" t="s">
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="20"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>1</v>
       </c>
@@ -4763,7 +4804,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -4777,7 +4818,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -4791,7 +4832,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -4805,7 +4846,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
@@ -4819,7 +4860,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
@@ -4833,31 +4874,31 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A28" s="19" t="s">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="20" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20" t="s">
+      <c r="B29" s="21"/>
+      <c r="C29" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="20"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
@@ -4871,7 +4912,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>2</v>
       </c>
@@ -4885,7 +4926,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -4899,7 +4940,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -4913,7 +4954,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -4927,7 +4968,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -4941,31 +4982,31 @@
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A37" s="21" t="s">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-    </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="20" t="s">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20" t="s">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="D38" s="20"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>1</v>
       </c>
@@ -4979,7 +5020,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>2</v>
       </c>
@@ -4993,7 +5034,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -5007,7 +5048,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -5021,7 +5062,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>5</v>
       </c>
@@ -5035,7 +5076,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>6</v>
       </c>
@@ -5049,31 +5090,31 @@
         <v>178</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
     </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A46" s="21" t="s">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-    </row>
-    <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="22" t="s">
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="20" t="s">
+      <c r="B47" s="20"/>
+      <c r="C47" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="D47" s="20"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>1</v>
       </c>
@@ -5087,7 +5128,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>2</v>
       </c>
@@ -5101,7 +5142,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -5115,7 +5156,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -5129,7 +5170,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>5</v>
       </c>
@@ -5143,7 +5184,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>6</v>
       </c>
@@ -5159,12 +5200,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -5177,6 +5212,12 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>